<commit_message>
add spares to bid act
</commit_message>
<xml_diff>
--- a/templates/excel/act/sample.xlsx
+++ b/templates/excel/act/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t xml:space="preserve">Приложение № 4  к Договору № ______  от «__» ______________ 20__г.</t>
   </si>
@@ -152,6 +152,48 @@
   </si>
   <si>
     <t xml:space="preserve">{job_total_price}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Название</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Артикул</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кол-во</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Всего</t>
+  </si>
+  <si>
+    <t xml:space="preserve">детали</t>
+  </si>
+  <si>
+    <t xml:space="preserve">деталей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_nom_row}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_vendor_code}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_quantity}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_price}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_total_price}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_quantity_all}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare_total_price_all}</t>
   </si>
   <si>
     <t xml:space="preserve">Ответственный сотрудник  сервисного центра           </t>
@@ -180,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -271,6 +313,12 @@
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -358,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -447,8 +495,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -459,7 +511,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,13 +596,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ45"/>
+  <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.17"/>
@@ -901,76 +957,150 @@
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
     </row>
-    <row r="34" s="17" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" s="18" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" s="18" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" s="18" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C36" s="18" t="s">
-        <v>44</v>
-      </c>
+    <row r="36" s="18" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="19"/>
+      <c r="AMH36" s="0"/>
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C37" s="18" t="s">
-        <v>45</v>
-      </c>
+    <row r="37" s="18" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="AMH37" s="0"/>
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C38" s="18" t="s">
-        <v>46</v>
+    <row r="38" s="17" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E38" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" s="18" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C40" s="18" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" s="24" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>49</v>
+    <row r="41" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C41" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" s="25" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C42" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" s="25" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="25" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C44" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" s="25" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" s="26" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>63</v>
+      </c>
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
+    <row r="46" s="27" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMI46" s="0"/>
+      <c r="AMJ46" s="0"/>
+    </row>
+    <row r="47" s="27" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMI47" s="0"/>
+      <c r="AMJ47" s="0"/>
+    </row>
+    <row r="48" s="27" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMI48" s="0"/>
+      <c r="AMJ48" s="0"/>
+    </row>
+    <row r="49" s="27" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMI49" s="0"/>
+      <c r="AMJ49" s="0"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="24">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C6:E6"/>
@@ -992,6 +1122,9 @@
     <mergeCell ref="D28:I28"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="E30:E31"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="G35:G36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.39375" bottom="0.39375" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>